<commit_message>
solve the new quiz and attach the 2 quizzes files
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,114 +434,129 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Age</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Score</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Alice</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>20</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Bob</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>21</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>85</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Charlie</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>19</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>David</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>22</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Eva</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>20</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>80</v>
       </c>
     </row>

</xml_diff>